<commit_message>
(NCIOCPL#80) Search Engine Restriction tests give a false failure.
Incidental: Change YAML content request to static content.
</commit_message>
<xml_diff>
--- a/test-data/searchenginerestrictions_data.xlsx
+++ b/test-data/searchenginerestrictions_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E9D360-707F-456D-A52A-E1E61044DD03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE70E61C-7B8E-2945-8371-D5B62D7B7EC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24460" yWindow="980" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getpages_with_index" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>path</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>Blog Post</t>
-  </si>
-  <si>
-    <t>/about-cancer/causes-prevention/vitamin-d-fact-sheet</t>
-  </si>
-  <si>
-    <t>/about-cancer/coping/self-image</t>
   </si>
 </sst>
 </file>
@@ -386,17 +380,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -418,7 +412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -429,7 +423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -448,19 +442,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD1206-3591-4D75-B37B-F40530826E59}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,28 +463,6 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tests for Citations
- Also adds Link class.
</commit_message>
<xml_diff>
--- a/test-data/searchenginerestrictions_data.xlsx
+++ b/test-data/searchenginerestrictions_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE70E61C-7B8E-2945-8371-D5B62D7B7EC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864F25A-E9EE-4808-8200-F3FD9523A852}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24460" yWindow="980" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24465" yWindow="975" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getpages_with_index" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>path</t>
   </si>
@@ -35,9 +35,6 @@
     <t>/about-cancer/coping/feelings/relaxation</t>
   </si>
   <si>
-    <t>article</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -51,6 +48,102 @@
   </si>
   <si>
     <t>Blog Post</t>
+  </si>
+  <si>
+    <t>/espanol/efectos-secundarios</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/comunicados-de-prensa/2018/leucemia-llc-ibrutinib-estudio</t>
+  </si>
+  <si>
+    <t>Press Release</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018/leukemia-cll-ibrutinib-trial</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>Blog Series</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/temas-y-relatos-blog</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/chanock-stephen</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/dfharvard</t>
+  </si>
+  <si>
+    <t>Cancer Center</t>
+  </si>
+  <si>
+    <t>/types/breast/research</t>
+  </si>
+  <si>
+    <t>Cancer Research List Page</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/seno/investigacion</t>
+  </si>
+  <si>
+    <t>/types/breast</t>
+  </si>
+  <si>
+    <t>Cancer Type Home Page</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/seno</t>
+  </si>
+  <si>
+    <t>/types/breast/hp</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/2019-investigators-site</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>/about-cancer</t>
+  </si>
+  <si>
+    <t>Home &amp; Landing</t>
+  </si>
+  <si>
+    <t>/espanol/cancer</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018</t>
+  </si>
+  <si>
+    <t>Mini Landing Page</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/comunicados-de-prensa/2018</t>
+  </si>
+  <si>
+    <t>/about-nci/organization/screen-to-save-infographic</t>
+  </si>
+  <si>
+    <t>Infographic</t>
+  </si>
+  <si>
+    <t>/espanol/infografia-nci</t>
+  </si>
+  <si>
+    <t>/research/progress/discovery/gutcheck-intro-video</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
@@ -377,20 +470,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,37 +494,257 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -444,17 +757,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD1206-3591-4D75-B37B-F40530826E59}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>